<commit_message>
Update to the nav so random and A-Z works
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam.todd/Documents/Work/jmu_work/graphic-design-and-illustration-2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7C31D8-40C2-2842-A7FD-677847A326BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AFA500-3FD8-F54E-BAB8-F8866C9445A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{EAD6A9B3-73FF-8A4D-B9DA-D03791ECC004}"/>
   </bookViews>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAB3878-818F-B441-9DC2-2B5ADF01F06F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B9"/>
+      <selection activeCell="B1" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,6 +461,14 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>